<commit_message>
Commit after yaml fixing.
</commit_message>
<xml_diff>
--- a/data/01_Sioux_Falls/minimum_input/standard_solution_link_performance_comparison.xlsx
+++ b/data/01_Sioux_Falls/minimum_input/standard_solution_link_performance_comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xzhou\source\repos\asu-trans-ai-lab\DTALite\data\01_Sioux_Falls\minimum_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF5531A-6CE5-4379-B324-D45ECF950AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CB32AF-11C5-45C0-9840-AD44C3895B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,232 +265,232 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="76"/>
                 <c:pt idx="0">
-                  <c:v>5940</c:v>
+                  <c:v>4853.085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7028</c:v>
+                  <c:v>8480.9599999999991</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4667</c:v>
+                  <c:v>4880.9589999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7750</c:v>
+                  <c:v>5805.2430000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8301</c:v>
+                  <c:v>8453.0849999999991</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7205</c:v>
+                  <c:v>14764.084999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4875</c:v>
+                  <c:v>10554.974</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8528</c:v>
+                  <c:v>14721.856</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4622</c:v>
+                  <c:v>18620.991999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11961</c:v>
+                  <c:v>5199.9799999999996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5301</c:v>
+                  <c:v>18690.870999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6311</c:v>
+                  <c:v>8595.5339999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6484</c:v>
+                  <c:v>15882.841</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6477</c:v>
+                  <c:v>5833.1170000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6990</c:v>
+                  <c:v>8629.0609999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10180</c:v>
+                  <c:v>12648.62</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13204</c:v>
+                  <c:v>12366.916999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6998</c:v>
+                  <c:v>15761.629000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9586</c:v>
+                  <c:v>12710.021000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14002</c:v>
+                  <c:v>12204.632</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11924</c:v>
+                  <c:v>6937.1940000000004</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>12002</c:v>
+                  <c:v>8378.8619999999992</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>6484</c:v>
+                  <c:v>15919.191999999999</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>12716</c:v>
+                  <c:v>6834.875</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22064</c:v>
+                  <c:v>22019.831999999999</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22956</c:v>
+                  <c:v>22053.863000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42154</c:v>
+                  <c:v>17674.623</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>31101</c:v>
+                  <c:v>23043.798999999999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13209</c:v>
+                  <c:v>11096.831</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>12326</c:v>
+                  <c:v>8100</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>12705</c:v>
+                  <c:v>5187.8739999999998</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>41489</c:v>
+                  <c:v>17625.607</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>18797</c:v>
+                  <c:v>8354.2209999999995</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>15440</c:v>
+                  <c:v>9773.91</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4825</c:v>
+                  <c:v>10569.326999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>18685</c:v>
+                  <c:v>8370.5959999999995</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>13232</c:v>
+                  <c:v>13057.752</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>13170</c:v>
+                  <c:v>13188.48</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>8458</c:v>
+                  <c:v>11001.966</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>15731</c:v>
+                  <c:v>9796.4130000000005</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5050</c:v>
+                  <c:v>8988.777</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9686</c:v>
+                  <c:v>8208.3960000000006</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>28820</c:v>
+                  <c:v>23011.469000000001</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5440</c:v>
+                  <c:v>9022.4390000000003</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10754</c:v>
+                  <c:v>18983.074000000001</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>17617</c:v>
+                  <c:v>18193.945</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>11414</c:v>
+                  <c:v>8380.2970000000005</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>16650</c:v>
+                  <c:v>11112.21</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9402</c:v>
+                  <c:v>11034.388000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5081</c:v>
+                  <c:v>16196.311</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>12623</c:v>
+                  <c:v>8100</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8814</c:v>
+                  <c:v>11160.094999999999</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>7018</c:v>
+                  <c:v>9556.4860000000008</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6200</c:v>
+                  <c:v>15923.913</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>8522</c:v>
+                  <c:v>16087.416999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9883</c:v>
+                  <c:v>19905.261999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7704</c:v>
+                  <c:v>18868.471000000001</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6727</c:v>
+                  <c:v>9682.1929999999993</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>10282</c:v>
+                  <c:v>8566.6229999999996</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>12426</c:v>
+                  <c:v>19858.651999999998</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6941</c:v>
+                  <c:v>8577.7279999999992</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>6946</c:v>
+                  <c:v>6205.0879999999997</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5003</c:v>
+                  <c:v>7067.018</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6840</c:v>
+                  <c:v>6119.9780000000001</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>8682</c:v>
+                  <c:v>8504.0619999999999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7326</c:v>
+                  <c:v>10222.262000000001</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>18676</c:v>
+                  <c:v>18209.879000000001</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4211</c:v>
+                  <c:v>7016.6239999999998</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>8118</c:v>
+                  <c:v>8489.5439999999999</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4112</c:v>
+                  <c:v>9551.4639999999999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>9587</c:v>
+                  <c:v>8197.2379999999994</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>3815</c:v>
+                  <c:v>9502.4860000000008</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>2334</c:v>
+                  <c:v>7846.116</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>8296</c:v>
+                  <c:v>11032.694</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>7784</c:v>
+                  <c:v>10151.669</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1938</c:v>
+                  <c:v>7785.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1777,13 +1777,13 @@
   <dimension ref="A1:R77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4"/>
   <cols>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="1"/>
+    <col min="14" max="14" width="8.88671875" style="1"/>
     <col min="18" max="18" width="12.88671875"/>
   </cols>
   <sheetData>
@@ -1869,7 +1869,7 @@
         <v>2</v>
       </c>
       <c r="N2" s="1">
-        <v>5940</v>
+        <v>4853.085</v>
       </c>
       <c r="O2">
         <v>5083.2139999999999</v>
@@ -1919,7 +1919,7 @@
         <v>3</v>
       </c>
       <c r="N3" s="1">
-        <v>7028</v>
+        <v>8480.9599999999991</v>
       </c>
       <c r="O3">
         <v>8782.6139999999996</v>
@@ -1969,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="1">
-        <v>4667</v>
+        <v>4880.9589999999998</v>
       </c>
       <c r="O4">
         <v>5182.6130000000003</v>
@@ -2019,7 +2019,7 @@
         <v>6</v>
       </c>
       <c r="N5" s="1">
-        <v>7750</v>
+        <v>5805.2430000000004</v>
       </c>
       <c r="O5">
         <v>5483.2139999999999</v>
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="1">
-        <v>8301</v>
+        <v>8453.0849999999991</v>
       </c>
       <c r="O6">
         <v>8683.2150000000001</v>
@@ -2119,7 +2119,7 @@
         <v>4</v>
       </c>
       <c r="N7" s="1">
-        <v>7205</v>
+        <v>14764.084999999999</v>
       </c>
       <c r="O7">
         <v>14796.576999999999</v>
@@ -2169,7 +2169,7 @@
         <v>12</v>
       </c>
       <c r="N8" s="1">
-        <v>4875</v>
+        <v>10554.974</v>
       </c>
       <c r="O8">
         <v>10373.788</v>
@@ -2219,7 +2219,7 @@
         <v>3</v>
       </c>
       <c r="N9" s="1">
-        <v>8528</v>
+        <v>14721.856</v>
       </c>
       <c r="O9">
         <v>14791.177</v>
@@ -2269,7 +2269,7 @@
         <v>5</v>
       </c>
       <c r="N10" s="1">
-        <v>4622</v>
+        <v>18620.991999999998</v>
       </c>
       <c r="O10">
         <v>18945.743999999999</v>
@@ -2319,7 +2319,7 @@
         <v>11</v>
       </c>
       <c r="N11" s="1">
-        <v>11961</v>
+        <v>5199.9799999999996</v>
       </c>
       <c r="O11">
         <v>5240.8310000000001</v>
@@ -2369,7 +2369,7 @@
         <v>4</v>
       </c>
       <c r="N12" s="1">
-        <v>5301</v>
+        <v>18690.870999999999</v>
       </c>
       <c r="O12">
         <v>18832.006000000001</v>
@@ -2419,7 +2419,7 @@
         <v>6</v>
       </c>
       <c r="N13" s="1">
-        <v>6311</v>
+        <v>8595.5339999999997</v>
       </c>
       <c r="O13">
         <v>8554.2849999999999</v>
@@ -2469,7 +2469,7 @@
         <v>9</v>
       </c>
       <c r="N14" s="1">
-        <v>6484</v>
+        <v>15882.841</v>
       </c>
       <c r="O14">
         <v>15714.925999999999</v>
@@ -2519,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="N15" s="1">
-        <v>6477</v>
+        <v>5833.1170000000002</v>
       </c>
       <c r="O15">
         <v>5582.6130000000003</v>
@@ -2569,7 +2569,7 @@
         <v>5</v>
       </c>
       <c r="N16" s="1">
-        <v>6990</v>
+        <v>8629.0609999999997</v>
       </c>
       <c r="O16">
         <v>8519.1620000000003</v>
@@ -2619,7 +2619,7 @@
         <v>8</v>
       </c>
       <c r="N17" s="1">
-        <v>10180</v>
+        <v>12648.62</v>
       </c>
       <c r="O17">
         <v>12837.499</v>
@@ -2669,7 +2669,7 @@
         <v>8</v>
       </c>
       <c r="N18" s="1">
-        <v>13204</v>
+        <v>12366.916999999999</v>
       </c>
       <c r="O18">
         <v>12616.312</v>
@@ -2719,7 +2719,7 @@
         <v>18</v>
       </c>
       <c r="N19" s="1">
-        <v>6998</v>
+        <v>15761.629000000001</v>
       </c>
       <c r="O19">
         <v>15620.555</v>
@@ -2769,7 +2769,7 @@
         <v>6</v>
       </c>
       <c r="N20" s="1">
-        <v>9586</v>
+        <v>12710.021000000001</v>
       </c>
       <c r="O20">
         <v>12901.775</v>
@@ -2819,7 +2819,7 @@
         <v>7</v>
       </c>
       <c r="N21" s="1">
-        <v>14002</v>
+        <v>12204.632</v>
       </c>
       <c r="O21">
         <v>12528.57</v>
@@ -2869,7 +2869,7 @@
         <v>9</v>
       </c>
       <c r="N22" s="1">
-        <v>11924</v>
+        <v>6937.1940000000004</v>
       </c>
       <c r="O22">
         <v>7211.1840000000002</v>
@@ -2919,7 +2919,7 @@
         <v>16</v>
       </c>
       <c r="N23" s="1">
-        <v>12002</v>
+        <v>8378.8619999999992</v>
       </c>
       <c r="O23">
         <v>8565.5689999999995</v>
@@ -2969,7 +2969,7 @@
         <v>5</v>
       </c>
       <c r="N24" s="1">
-        <v>6484</v>
+        <v>15919.191999999999</v>
       </c>
       <c r="O24">
         <v>15636.311</v>
@@ -3019,7 +3019,7 @@
         <v>8</v>
       </c>
       <c r="N25" s="1">
-        <v>12716</v>
+        <v>6834.875</v>
       </c>
       <c r="O25">
         <v>7156.6409999999996</v>
@@ -3069,7 +3069,7 @@
         <v>10</v>
       </c>
       <c r="N26" s="1">
-        <v>22064</v>
+        <v>22019.831999999999</v>
       </c>
       <c r="O26">
         <v>21936.92</v>
@@ -3119,7 +3119,7 @@
         <v>9</v>
       </c>
       <c r="N27" s="1">
-        <v>22956</v>
+        <v>22053.863000000001</v>
       </c>
       <c r="O27">
         <v>21903.759999999998</v>
@@ -3169,7 +3169,7 @@
         <v>11</v>
       </c>
       <c r="N28" s="1">
-        <v>42154</v>
+        <v>17674.623</v>
       </c>
       <c r="O28">
         <v>17616.918000000001</v>
@@ -3219,7 +3219,7 @@
         <v>15</v>
       </c>
       <c r="N29" s="1">
-        <v>31101</v>
+        <v>23043.798999999999</v>
       </c>
       <c r="O29">
         <v>22471.785</v>
@@ -3269,7 +3269,7 @@
         <v>16</v>
       </c>
       <c r="N30" s="1">
-        <v>13209</v>
+        <v>11096.831</v>
       </c>
       <c r="O30">
         <v>11370.813</v>
@@ -3319,7 +3319,7 @@
         <v>17</v>
       </c>
       <c r="N31" s="1">
-        <v>12326</v>
+        <v>8100</v>
       </c>
       <c r="O31">
         <v>8099.9989999999998</v>
@@ -3369,7 +3369,7 @@
         <v>4</v>
       </c>
       <c r="N32" s="1">
-        <v>12705</v>
+        <v>5187.8739999999998</v>
       </c>
       <c r="O32">
         <v>5449.17</v>
@@ -3419,7 +3419,7 @@
         <v>10</v>
       </c>
       <c r="N33" s="1">
-        <v>41489</v>
+        <v>17625.607</v>
       </c>
       <c r="O33">
         <v>17464.998</v>
@@ -3469,7 +3469,7 @@
         <v>12</v>
       </c>
       <c r="N34" s="1">
-        <v>18797</v>
+        <v>8354.2209999999995</v>
       </c>
       <c r="O34">
         <v>8377.5220000000008</v>
@@ -3519,7 +3519,7 @@
         <v>14</v>
       </c>
       <c r="N35" s="1">
-        <v>15440</v>
+        <v>9773.91</v>
       </c>
       <c r="O35">
         <v>9587.5490000000009</v>
@@ -3569,7 +3569,7 @@
         <v>3</v>
       </c>
       <c r="N36" s="1">
-        <v>4825</v>
+        <v>10569.326999999999</v>
       </c>
       <c r="O36">
         <v>10279.791999999999</v>
@@ -3619,7 +3619,7 @@
         <v>11</v>
       </c>
       <c r="N37" s="1">
-        <v>18685</v>
+        <v>8370.5959999999995</v>
       </c>
       <c r="O37">
         <v>8460.4220000000005</v>
@@ -3669,7 +3669,7 @@
         <v>13</v>
       </c>
       <c r="N38" s="1">
-        <v>13232</v>
+        <v>13057.752</v>
       </c>
       <c r="O38">
         <v>13227.405000000001</v>
@@ -3719,7 +3719,7 @@
         <v>12</v>
       </c>
       <c r="N39" s="1">
-        <v>13170</v>
+        <v>13188.48</v>
       </c>
       <c r="O39">
         <v>13316.306</v>
@@ -3769,7 +3769,7 @@
         <v>24</v>
       </c>
       <c r="N40" s="1">
-        <v>8458</v>
+        <v>11001.966</v>
       </c>
       <c r="O40">
         <v>10975.704</v>
@@ -3819,7 +3819,7 @@
         <v>11</v>
       </c>
       <c r="N41" s="1">
-        <v>15731</v>
+        <v>9796.4130000000005</v>
       </c>
       <c r="O41">
         <v>9661.0709999999999</v>
@@ -3869,7 +3869,7 @@
         <v>15</v>
       </c>
       <c r="N42" s="1">
-        <v>5050</v>
+        <v>8988.777</v>
       </c>
       <c r="O42">
         <v>8967.3150000000005</v>
@@ -3919,7 +3919,7 @@
         <v>23</v>
       </c>
       <c r="N43" s="1">
-        <v>9686</v>
+        <v>8208.3960000000006</v>
       </c>
       <c r="O43">
         <v>8224.4509999999991</v>
@@ -3969,7 +3969,7 @@
         <v>10</v>
       </c>
       <c r="N44" s="1">
-        <v>28820</v>
+        <v>23011.469000000001</v>
       </c>
       <c r="O44">
         <v>22484.833999999999</v>
@@ -4019,7 +4019,7 @@
         <v>14</v>
       </c>
       <c r="N45" s="1">
-        <v>5440</v>
+        <v>9022.4390000000003</v>
       </c>
       <c r="O45">
         <v>9041.5010000000002</v>
@@ -4069,7 +4069,7 @@
         <v>19</v>
       </c>
       <c r="N46" s="1">
-        <v>10754</v>
+        <v>18983.074000000001</v>
       </c>
       <c r="O46">
         <v>17955.973000000002</v>
@@ -4119,7 +4119,7 @@
         <v>22</v>
       </c>
       <c r="N47" s="1">
-        <v>17617</v>
+        <v>18193.945</v>
       </c>
       <c r="O47">
         <v>18078.322</v>
@@ -4169,7 +4169,7 @@
         <v>8</v>
       </c>
       <c r="N48" s="1">
-        <v>11414</v>
+        <v>8380.2970000000005</v>
       </c>
       <c r="O48">
         <v>8596.6460000000006</v>
@@ -4219,7 +4219,7 @@
         <v>10</v>
       </c>
       <c r="N49" s="1">
-        <v>16650</v>
+        <v>11112.21</v>
       </c>
       <c r="O49">
         <v>11376.53</v>
@@ -4269,7 +4269,7 @@
         <v>17</v>
       </c>
       <c r="N50" s="1">
-        <v>9402</v>
+        <v>11034.388000000001</v>
       </c>
       <c r="O50">
         <v>10895.549000000001</v>
@@ -4319,7 +4319,7 @@
         <v>18</v>
       </c>
       <c r="N51" s="1">
-        <v>5081</v>
+        <v>16196.311</v>
       </c>
       <c r="O51">
         <v>16700.59</v>
@@ -4369,7 +4369,7 @@
         <v>10</v>
       </c>
       <c r="N52" s="1">
-        <v>12623</v>
+        <v>8100</v>
       </c>
       <c r="O52">
         <v>8099.9989999999998</v>
@@ -4419,7 +4419,7 @@
         <v>16</v>
       </c>
       <c r="N53" s="1">
-        <v>8814</v>
+        <v>11160.094999999999</v>
       </c>
       <c r="O53">
         <v>10905.317999999999</v>
@@ -4469,7 +4469,7 @@
         <v>19</v>
       </c>
       <c r="N54" s="1">
-        <v>7018</v>
+        <v>9556.4860000000008</v>
       </c>
       <c r="O54">
         <v>9948.7530000000006</v>
@@ -4519,7 +4519,7 @@
         <v>7</v>
       </c>
       <c r="N55" s="1">
-        <v>6200</v>
+        <v>15923.913</v>
       </c>
       <c r="O55">
         <v>15708.296</v>
@@ -4569,7 +4569,7 @@
         <v>16</v>
       </c>
       <c r="N56" s="1">
-        <v>8522</v>
+        <v>16087.416999999999</v>
       </c>
       <c r="O56">
         <v>16727.611000000001</v>
@@ -4619,7 +4619,7 @@
         <v>20</v>
       </c>
       <c r="N57" s="1">
-        <v>9883</v>
+        <v>19905.261999999999</v>
       </c>
       <c r="O57">
         <v>20692.294999999998</v>
@@ -4669,7 +4669,7 @@
         <v>15</v>
       </c>
       <c r="N58" s="1">
-        <v>7704</v>
+        <v>18868.471000000001</v>
       </c>
       <c r="O58">
         <v>17964.596000000001</v>
@@ -4719,7 +4719,7 @@
         <v>17</v>
       </c>
       <c r="N59" s="1">
-        <v>6727</v>
+        <v>9682.1929999999993</v>
       </c>
       <c r="O59">
         <v>9958.5249999999996</v>
@@ -4769,7 +4769,7 @@
         <v>20</v>
       </c>
       <c r="N60" s="1">
-        <v>10282</v>
+        <v>8566.6229999999996</v>
       </c>
       <c r="O60">
         <v>7899.5450000000001</v>
@@ -4819,7 +4819,7 @@
         <v>18</v>
       </c>
       <c r="N61" s="1">
-        <v>12426</v>
+        <v>19858.651999999998</v>
       </c>
       <c r="O61">
         <v>20707.057000000001</v>
@@ -4869,7 +4869,7 @@
         <v>19</v>
       </c>
       <c r="N62" s="1">
-        <v>6941</v>
+        <v>8577.7279999999992</v>
       </c>
       <c r="O62">
         <v>7917.9369999999999</v>
@@ -4919,7 +4919,7 @@
         <v>21</v>
       </c>
       <c r="N63" s="1">
-        <v>6946</v>
+        <v>6205.0879999999997</v>
       </c>
       <c r="O63">
         <v>6445.915</v>
@@ -4969,7 +4969,7 @@
         <v>22</v>
       </c>
       <c r="N64" s="1">
-        <v>5003</v>
+        <v>7067.018</v>
       </c>
       <c r="O64">
         <v>7000</v>
@@ -5019,7 +5019,7 @@
         <v>20</v>
       </c>
       <c r="N65" s="1">
-        <v>6840</v>
+        <v>6119.9780000000001</v>
       </c>
       <c r="O65">
         <v>6379.0690000000004</v>
@@ -5069,7 +5069,7 @@
         <v>22</v>
       </c>
       <c r="N66" s="1">
-        <v>8682</v>
+        <v>8504.0619999999999</v>
       </c>
       <c r="O66">
         <v>8315.6170000000002</v>
@@ -5119,7 +5119,7 @@
         <v>24</v>
       </c>
       <c r="N67" s="1">
-        <v>7326</v>
+        <v>10222.262000000001</v>
       </c>
       <c r="O67">
         <v>10299.105</v>
@@ -5169,7 +5169,7 @@
         <v>15</v>
       </c>
       <c r="N68" s="1">
-        <v>18676</v>
+        <v>18209.879000000001</v>
       </c>
       <c r="O68">
         <v>18056.934000000001</v>
@@ -5219,7 +5219,7 @@
         <v>20</v>
       </c>
       <c r="N69" s="1">
-        <v>4211</v>
+        <v>7016.6239999999998</v>
       </c>
       <c r="O69">
         <v>7000</v>
@@ -5269,7 +5269,7 @@
         <v>21</v>
       </c>
       <c r="N70" s="1">
-        <v>8118</v>
+        <v>8489.5439999999999</v>
       </c>
       <c r="O70">
         <v>8299.4609999999993</v>
@@ -5319,7 +5319,7 @@
         <v>23</v>
       </c>
       <c r="N71" s="1">
-        <v>4112</v>
+        <v>9551.4639999999999</v>
       </c>
       <c r="O71">
         <v>9604.3880000000008</v>
@@ -5369,7 +5369,7 @@
         <v>14</v>
       </c>
       <c r="N72" s="1">
-        <v>9587</v>
+        <v>8197.2379999999994</v>
       </c>
       <c r="O72">
         <v>8223.7860000000001</v>
@@ -5419,7 +5419,7 @@
         <v>22</v>
       </c>
       <c r="N73" s="1">
-        <v>3815</v>
+        <v>9502.4860000000008</v>
       </c>
       <c r="O73">
         <v>9566.8430000000008</v>
@@ -5469,7 +5469,7 @@
         <v>24</v>
       </c>
       <c r="N74" s="1">
-        <v>2334</v>
+        <v>7846.116</v>
       </c>
       <c r="O74">
         <v>7742.6930000000002</v>
@@ -5519,7 +5519,7 @@
         <v>13</v>
       </c>
       <c r="N75" s="1">
-        <v>8296</v>
+        <v>11032.694</v>
       </c>
       <c r="O75">
         <v>10964.603999999999</v>
@@ -5569,7 +5569,7 @@
         <v>21</v>
       </c>
       <c r="N76" s="1">
-        <v>7784</v>
+        <v>10151.669</v>
       </c>
       <c r="O76">
         <v>10248.416999999999</v>
@@ -5619,7 +5619,7 @@
         <v>23</v>
       </c>
       <c r="N77" s="1">
-        <v>1938</v>
+        <v>7785.98</v>
       </c>
       <c r="O77">
         <v>7704.4809999999998</v>

</xml_diff>